<commit_message>
Chỉnh sửa file đầu vào
</commit_message>
<xml_diff>
--- a/Template/DV3.xlsx
+++ b/Template/DV3.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="58">
   <si>
     <t xml:space="preserve">KẾ HOẠCH KIỂM TOÁN </t>
   </si>
@@ -61,9 +61,6 @@
     <t>BCTC</t>
   </si>
   <si>
-    <t>HC Toàn Cầu</t>
-  </si>
-  <si>
     <t>XMT</t>
   </si>
   <si>
@@ -73,33 +70,18 @@
     <t>NVB</t>
   </si>
   <si>
-    <t>Nhựa Bình Minh MB</t>
-  </si>
-  <si>
-    <t>19/12</t>
-  </si>
-  <si>
-    <t>SunZex</t>
-  </si>
-  <si>
     <t>NGUYỄN VĂN C</t>
   </si>
   <si>
     <t>NVC</t>
   </si>
   <si>
-    <t>Văn phòng đường sắt SG</t>
-  </si>
-  <si>
     <t>NGUYỄN VĂN D</t>
   </si>
   <si>
     <t>NVD</t>
   </si>
   <si>
-    <t>XMC - Chi nhánh Miền Nam</t>
-  </si>
-  <si>
     <t>NGUYỄN VĂN E</t>
   </si>
   <si>
@@ -115,9 +97,6 @@
     <t>NVF</t>
   </si>
   <si>
-    <t>Phoenix</t>
-  </si>
-  <si>
     <t>NGUYỄN VĂN G</t>
   </si>
   <si>
@@ -185,6 +164,36 @@
   </si>
   <si>
     <t>NVQ</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>CDF</t>
+  </si>
+  <si>
+    <t>ILM</t>
+  </si>
+  <si>
+    <t>MEY</t>
+  </si>
+  <si>
+    <t>HNO</t>
+  </si>
+  <si>
+    <t>LUO</t>
+  </si>
+  <si>
+    <t>MNO</t>
+  </si>
+  <si>
+    <t>HIK</t>
+  </si>
+  <si>
+    <t>XYV</t>
+  </si>
+  <si>
+    <t>KUY</t>
   </si>
 </sst>
 </file>
@@ -421,7 +430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -429,9 +438,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -444,22 +450,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -538,9 +529,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -549,6 +537,24 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3883,7 +3889,7 @@
   <dimension ref="A1:AF24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:C23"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3896,1782 +3902,1782 @@
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4" t="s">
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4" t="s">
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
+      <c r="S1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4" t="s">
+      <c r="T1" s="41"/>
+      <c r="U1" s="41"/>
+      <c r="V1" s="41"/>
+      <c r="W1" s="41"/>
+      <c r="X1" s="41"/>
+      <c r="Y1" s="41"/>
+      <c r="Z1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4"/>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="4"/>
+      <c r="AA1" s="41"/>
+      <c r="AB1" s="41"/>
+      <c r="AC1" s="41"/>
+      <c r="AD1" s="41"/>
+      <c r="AE1" s="41"/>
+      <c r="AF1" s="41"/>
     </row>
     <row r="2" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="6">
+      <c r="F2" s="5">
         <f>E4</f>
         <v>43465</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <f>J4</f>
         <v>43470</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="5" t="s">
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="5">
         <f>L4</f>
         <v>43472</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="6">
+      <c r="O2" s="5">
         <f>Q4</f>
         <v>43477</v>
       </c>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="5" t="s">
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="T2" s="6">
+      <c r="T2" s="5">
         <f>S4</f>
         <v>43479</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="U2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="V2" s="6">
+      <c r="V2" s="5">
         <f>X4</f>
         <v>43484</v>
       </c>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="5" t="s">
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="AA2" s="6">
+      <c r="AA2" s="5">
         <f>Z4</f>
         <v>43486</v>
       </c>
-      <c r="AB2" s="7" t="s">
+      <c r="AB2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="AC2" s="6">
+      <c r="AC2" s="5">
         <f>AE4</f>
         <v>43491</v>
       </c>
-      <c r="AD2" s="6"/>
-      <c r="AE2" s="6"/>
-      <c r="AF2" s="6"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="8"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="8"/>
-      <c r="AA3" s="8"/>
-      <c r="AB3" s="8"/>
-      <c r="AC3" s="8"/>
-      <c r="AD3" s="8"/>
-      <c r="AE3" s="8"/>
-      <c r="AF3" s="8"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="7"/>
+      <c r="AE3" s="7"/>
+      <c r="AF3" s="7"/>
     </row>
     <row r="4" spans="1:32" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="9">
         <v>43465</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="9">
         <f t="shared" ref="F4:AF4" si="0">E4+1</f>
         <v>43466</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="9">
         <f t="shared" si="0"/>
         <v>43467</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="9">
         <f t="shared" si="0"/>
         <v>43468</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="9">
         <f t="shared" si="0"/>
         <v>43469</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="9">
         <f t="shared" si="0"/>
         <v>43470</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="9">
         <f t="shared" si="0"/>
         <v>43471</v>
       </c>
-      <c r="L4" s="12">
+      <c r="L4" s="9">
         <f t="shared" si="0"/>
         <v>43472</v>
       </c>
-      <c r="M4" s="12">
+      <c r="M4" s="9">
         <f t="shared" si="0"/>
         <v>43473</v>
       </c>
-      <c r="N4" s="12">
+      <c r="N4" s="9">
         <f t="shared" si="0"/>
         <v>43474</v>
       </c>
-      <c r="O4" s="12">
+      <c r="O4" s="9">
         <f t="shared" si="0"/>
         <v>43475</v>
       </c>
-      <c r="P4" s="12">
+      <c r="P4" s="9">
         <f t="shared" si="0"/>
         <v>43476</v>
       </c>
-      <c r="Q4" s="12">
+      <c r="Q4" s="9">
         <f t="shared" si="0"/>
         <v>43477</v>
       </c>
-      <c r="R4" s="12">
+      <c r="R4" s="9">
         <f t="shared" si="0"/>
         <v>43478</v>
       </c>
-      <c r="S4" s="12">
+      <c r="S4" s="9">
         <f t="shared" si="0"/>
         <v>43479</v>
       </c>
-      <c r="T4" s="12">
+      <c r="T4" s="9">
         <f t="shared" si="0"/>
         <v>43480</v>
       </c>
-      <c r="U4" s="12">
+      <c r="U4" s="9">
         <f t="shared" si="0"/>
         <v>43481</v>
       </c>
-      <c r="V4" s="12">
+      <c r="V4" s="9">
         <f t="shared" si="0"/>
         <v>43482</v>
       </c>
-      <c r="W4" s="12">
+      <c r="W4" s="9">
         <f t="shared" si="0"/>
         <v>43483</v>
       </c>
-      <c r="X4" s="12">
+      <c r="X4" s="9">
         <f t="shared" si="0"/>
         <v>43484</v>
       </c>
-      <c r="Y4" s="12">
+      <c r="Y4" s="9">
         <f t="shared" si="0"/>
         <v>43485</v>
       </c>
-      <c r="Z4" s="12">
+      <c r="Z4" s="9">
         <f t="shared" si="0"/>
         <v>43486</v>
       </c>
-      <c r="AA4" s="12">
+      <c r="AA4" s="9">
         <f t="shared" si="0"/>
         <v>43487</v>
       </c>
-      <c r="AB4" s="12">
+      <c r="AB4" s="9">
         <f t="shared" si="0"/>
         <v>43488</v>
       </c>
-      <c r="AC4" s="12">
+      <c r="AC4" s="9">
         <f t="shared" si="0"/>
         <v>43489</v>
       </c>
-      <c r="AD4" s="12">
+      <c r="AD4" s="9">
         <f t="shared" si="0"/>
         <v>43490</v>
       </c>
-      <c r="AE4" s="12">
+      <c r="AE4" s="9">
         <f t="shared" si="0"/>
         <v>43491</v>
       </c>
-      <c r="AF4" s="12">
+      <c r="AF4" s="9">
         <f t="shared" si="0"/>
         <v>43492</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="16">
+      <c r="A5" s="43"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="10">
         <v>2</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="10">
         <v>3</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="10">
         <v>4</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="10">
         <v>5</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="10">
         <v>6</v>
       </c>
-      <c r="J5" s="16">
+      <c r="J5" s="10">
         <v>7</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="K5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="16">
+      <c r="L5" s="10">
         <v>2</v>
       </c>
-      <c r="M5" s="16">
+      <c r="M5" s="10">
         <v>3</v>
       </c>
-      <c r="N5" s="16">
+      <c r="N5" s="10">
         <v>4</v>
       </c>
-      <c r="O5" s="16">
+      <c r="O5" s="10">
         <v>5</v>
       </c>
-      <c r="P5" s="16">
+      <c r="P5" s="10">
         <v>6</v>
       </c>
-      <c r="Q5" s="16">
+      <c r="Q5" s="10">
         <v>7</v>
       </c>
-      <c r="R5" s="16" t="s">
+      <c r="R5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="S5" s="16">
+      <c r="S5" s="10">
         <v>2</v>
       </c>
-      <c r="T5" s="16">
+      <c r="T5" s="10">
         <v>3</v>
       </c>
-      <c r="U5" s="16">
+      <c r="U5" s="10">
         <v>4</v>
       </c>
-      <c r="V5" s="16">
+      <c r="V5" s="10">
         <v>5</v>
       </c>
-      <c r="W5" s="16">
+      <c r="W5" s="10">
         <v>6</v>
       </c>
-      <c r="X5" s="16">
+      <c r="X5" s="10">
         <v>7</v>
       </c>
-      <c r="Y5" s="16" t="s">
+      <c r="Y5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="Z5" s="16">
+      <c r="Z5" s="10">
         <v>2</v>
       </c>
-      <c r="AA5" s="16">
+      <c r="AA5" s="10">
         <v>3</v>
       </c>
-      <c r="AB5" s="16">
+      <c r="AB5" s="10">
         <v>4</v>
       </c>
-      <c r="AC5" s="16">
+      <c r="AC5" s="10">
         <v>5</v>
       </c>
-      <c r="AD5" s="16">
+      <c r="AD5" s="10">
         <v>6</v>
       </c>
-      <c r="AE5" s="16">
+      <c r="AE5" s="10">
         <v>7</v>
       </c>
-      <c r="AF5" s="16" t="s">
+      <c r="AF5" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="20"/>
-      <c r="R6" s="20"/>
-      <c r="S6" s="20"/>
-      <c r="T6" s="20"/>
-      <c r="U6" s="20"/>
-      <c r="V6" s="21"/>
-      <c r="W6" s="20"/>
-      <c r="X6" s="20"/>
-      <c r="Y6" s="20"/>
-      <c r="Z6" s="20"/>
-      <c r="AA6" s="20"/>
-      <c r="AB6" s="20"/>
-      <c r="AC6" s="21"/>
-      <c r="AD6" s="20"/>
-      <c r="AE6" s="20"/>
-      <c r="AF6" s="20"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="14"/>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="14"/>
+      <c r="AB6" s="14"/>
+      <c r="AC6" s="15"/>
+      <c r="AD6" s="14"/>
+      <c r="AE6" s="14"/>
+      <c r="AF6" s="14"/>
     </row>
     <row r="7" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21">
+      <c r="A7" s="15">
         <v>1</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="26"/>
-      <c r="L7" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="M7" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="N7" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="O7" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="P7" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q7" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="R7" s="26"/>
-      <c r="S7" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="T7" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="U7" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="V7" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="W7" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="X7" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="Y7" s="26"/>
-      <c r="Z7" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA7" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB7" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC7" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD7" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE7" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="AF7" s="26"/>
+      <c r="E7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" s="20"/>
+      <c r="L7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="M7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="N7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="O7" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="P7" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q7" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="R7" s="20"/>
+      <c r="S7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="T7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="U7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="V7" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="W7" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="X7" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y7" s="20"/>
+      <c r="Z7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC7" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD7" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE7" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF7" s="20"/>
     </row>
     <row r="8" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21">
+      <c r="A8" s="15">
         <f>A7+1</f>
         <v>2</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="K8" s="30"/>
-      <c r="L8" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="M8" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="N8" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="O8" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="P8" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q8" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="R8" s="30"/>
-      <c r="S8" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="T8" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="U8" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="V8" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="W8" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="X8" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y8" s="30"/>
-      <c r="Z8" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA8" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="AB8" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="AC8" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="AD8" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE8" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF8" s="30"/>
+      <c r="E8" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8" s="24"/>
+      <c r="L8" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="M8" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="N8" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="O8" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="P8" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q8" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="R8" s="24"/>
+      <c r="S8" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="T8" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="U8" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="V8" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="W8" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="X8" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y8" s="24"/>
+      <c r="Z8" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA8" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB8" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC8" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD8" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE8" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF8" s="24"/>
     </row>
     <row r="9" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21">
+      <c r="A9" s="15">
         <f t="shared" ref="A9:A14" si="1">A8+1</f>
         <v>3</v>
       </c>
-      <c r="B9" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="23" t="s">
+      <c r="B9" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" s="32"/>
-      <c r="L9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="M9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="N9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="O9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="P9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="R9" s="32"/>
-      <c r="S9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="T9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="U9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="V9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="W9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="X9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y9" s="32"/>
-      <c r="Z9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF9" s="32"/>
+      <c r="E9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="J9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="K9" s="26"/>
+      <c r="L9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="M9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="N9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="O9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="P9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="R9" s="26"/>
+      <c r="S9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="T9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="U9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="V9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="W9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="X9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y9" s="26"/>
+      <c r="Z9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF9" s="26"/>
     </row>
     <row r="10" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21">
+      <c r="A10" s="15">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B10" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="23" t="s">
+      <c r="B10" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="J10" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
-      <c r="O10" s="30"/>
-      <c r="P10" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q10" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="R10" s="30"/>
-      <c r="S10" s="30"/>
-      <c r="T10" s="30"/>
-      <c r="U10" s="30"/>
-      <c r="V10" s="30"/>
-      <c r="W10" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="X10" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y10" s="30"/>
-      <c r="Z10" s="30"/>
-      <c r="AA10" s="30"/>
-      <c r="AB10" s="30"/>
-      <c r="AC10" s="30"/>
-      <c r="AD10" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="AE10" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="AF10" s="30"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="J10" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q10" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="24"/>
+      <c r="U10" s="24"/>
+      <c r="V10" s="24"/>
+      <c r="W10" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="X10" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y10" s="24"/>
+      <c r="Z10" s="24"/>
+      <c r="AA10" s="24"/>
+      <c r="AB10" s="24"/>
+      <c r="AC10" s="24"/>
+      <c r="AD10" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE10" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF10" s="24"/>
     </row>
     <row r="11" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21">
+      <c r="A11" s="15">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B11" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="23" t="s">
+      <c r="B11" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="K11" s="32"/>
-      <c r="L11" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="M11" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="N11" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="O11" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="P11" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q11" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="R11" s="32"/>
-      <c r="S11" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="T11" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="U11" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="V11" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="W11" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="X11" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y11" s="32"/>
-      <c r="Z11" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA11" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB11" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC11" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD11" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE11" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF11" s="32"/>
+      <c r="E11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="26"/>
+      <c r="L11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="M11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="N11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="O11" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="P11" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q11" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="R11" s="26"/>
+      <c r="S11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="T11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="U11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="V11" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="W11" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="X11" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y11" s="26"/>
+      <c r="Z11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC11" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD11" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE11" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF11" s="26"/>
     </row>
     <row r="12" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21">
+      <c r="A12" s="15">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B12" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="23" t="s">
+      <c r="B12" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" s="30"/>
-      <c r="L12" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="M12" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="N12" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="O12" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="P12" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q12" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="R12" s="30"/>
-      <c r="S12" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="T12" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="U12" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="V12" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="W12" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="X12" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="Y12" s="30"/>
-      <c r="Z12" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA12" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB12" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC12" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD12" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE12" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="AF12" s="30"/>
+      <c r="E12" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="J12" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="K12" s="24"/>
+      <c r="L12" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="M12" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="N12" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="O12" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="P12" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q12" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="R12" s="24"/>
+      <c r="S12" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="T12" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="U12" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="V12" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="W12" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="X12" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y12" s="24"/>
+      <c r="Z12" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA12" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB12" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC12" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD12" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE12" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF12" s="24"/>
     </row>
     <row r="13" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21">
+      <c r="A13" s="15">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B13" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="23" t="s">
+      <c r="B13" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="I13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="J13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="K13" s="30"/>
-      <c r="L13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="M13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="N13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="O13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="P13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="R13" s="30"/>
-      <c r="S13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="T13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="U13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="V13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="W13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="X13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y13" s="30"/>
-      <c r="Z13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE13" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF13" s="30"/>
+      <c r="E13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="J13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="K13" s="24"/>
+      <c r="L13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="M13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="N13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="O13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="P13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="R13" s="24"/>
+      <c r="S13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="T13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="U13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="V13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="W13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="X13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y13" s="24"/>
+      <c r="Z13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE13" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF13" s="24"/>
     </row>
     <row r="14" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="21">
+      <c r="A14" s="15">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B14" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="23" t="s">
+      <c r="B14" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="30"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="30"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="M14" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="N14" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="O14" s="30"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="32"/>
-      <c r="S14" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="T14" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="U14" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="V14" s="30"/>
-      <c r="W14" s="30"/>
-      <c r="X14" s="30"/>
-      <c r="Y14" s="32"/>
-      <c r="Z14" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA14" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB14" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC14" s="30"/>
-      <c r="AD14" s="30"/>
-      <c r="AE14" s="30"/>
-      <c r="AF14" s="32"/>
+      <c r="E14" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="M14" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="N14" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="O14" s="24"/>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="26"/>
+      <c r="S14" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="T14" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="U14" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="V14" s="24"/>
+      <c r="W14" s="24"/>
+      <c r="X14" s="24"/>
+      <c r="Y14" s="26"/>
+      <c r="Z14" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA14" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB14" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC14" s="24"/>
+      <c r="AD14" s="24"/>
+      <c r="AE14" s="24"/>
+      <c r="AF14" s="26"/>
     </row>
     <row r="15" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21">
+      <c r="A15" s="15">
         <v>10</v>
       </c>
-      <c r="B15" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="23" t="s">
+      <c r="B15" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="J15" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="K15" s="32"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="30"/>
-      <c r="O15" s="30"/>
-      <c r="P15" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q15" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="R15" s="32"/>
-      <c r="S15" s="30"/>
-      <c r="T15" s="30"/>
-      <c r="U15" s="30"/>
-      <c r="V15" s="30"/>
-      <c r="W15" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="X15" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y15" s="32"/>
-      <c r="Z15" s="30"/>
-      <c r="AA15" s="30"/>
-      <c r="AB15" s="30"/>
-      <c r="AC15" s="30"/>
-      <c r="AD15" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="AE15" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="AF15" s="32"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="J15" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="K15" s="26"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q15" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="R15" s="26"/>
+      <c r="S15" s="24"/>
+      <c r="T15" s="24"/>
+      <c r="U15" s="24"/>
+      <c r="V15" s="24"/>
+      <c r="W15" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="X15" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y15" s="26"/>
+      <c r="Z15" s="24"/>
+      <c r="AA15" s="24"/>
+      <c r="AB15" s="24"/>
+      <c r="AC15" s="24"/>
+      <c r="AD15" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE15" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF15" s="26"/>
     </row>
     <row r="16" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21">
+      <c r="A16" s="15">
         <v>11</v>
       </c>
-      <c r="B16" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="23" t="s">
+      <c r="B16" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="J16" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="K16" s="32"/>
-      <c r="L16" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="M16" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="N16" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="O16" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="P16" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q16" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="R16" s="32"/>
-      <c r="S16" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="T16" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="U16" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="V16" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="W16" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="X16" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y16" s="32"/>
-      <c r="Z16" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA16" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB16" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC16" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD16" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE16" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF16" s="32"/>
+      <c r="E16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="H16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="I16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="J16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" s="26"/>
+      <c r="L16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="M16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="N16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="O16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="P16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="R16" s="26"/>
+      <c r="S16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="T16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="U16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="V16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="W16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="X16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y16" s="26"/>
+      <c r="Z16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE16" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF16" s="26"/>
     </row>
     <row r="17" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21">
+      <c r="A17" s="15">
         <f>A16+1</f>
         <v>12</v>
       </c>
-      <c r="B17" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="23" t="s">
+      <c r="B17" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="H17" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="J17" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="K17" s="30"/>
-      <c r="L17" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="M17" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="N17" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="O17" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="P17" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q17" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="R17" s="30"/>
-      <c r="S17" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="T17" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="U17" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="V17" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="W17" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="X17" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y17" s="30"/>
-      <c r="Z17" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA17" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AB17" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC17" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD17" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE17" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF17" s="30"/>
+      <c r="E17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="I17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="J17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="K17" s="24"/>
+      <c r="L17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="M17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="N17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="O17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="P17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="R17" s="24"/>
+      <c r="S17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="T17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="U17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="V17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="W17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="X17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y17" s="24"/>
+      <c r="Z17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE17" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF17" s="24"/>
     </row>
-    <row r="18" spans="1:32" s="38" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="37"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="37"/>
-      <c r="N18" s="37"/>
-      <c r="O18" s="37"/>
-      <c r="P18" s="37"/>
-      <c r="Q18" s="37"/>
-      <c r="R18" s="37"/>
-      <c r="S18" s="36"/>
-      <c r="T18" s="37"/>
-      <c r="U18" s="37"/>
-      <c r="V18" s="37"/>
-      <c r="W18" s="37"/>
-      <c r="X18" s="37"/>
-      <c r="Y18" s="37"/>
-      <c r="Z18" s="36"/>
-      <c r="AA18" s="37"/>
-      <c r="AB18" s="37"/>
-      <c r="AC18" s="37"/>
-      <c r="AD18" s="37"/>
-      <c r="AE18" s="37"/>
-      <c r="AF18" s="37"/>
+    <row r="18" spans="1:32" s="32" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="31"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="30"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="31"/>
+      <c r="P18" s="31"/>
+      <c r="Q18" s="31"/>
+      <c r="R18" s="31"/>
+      <c r="S18" s="30"/>
+      <c r="T18" s="31"/>
+      <c r="U18" s="31"/>
+      <c r="V18" s="31"/>
+      <c r="W18" s="31"/>
+      <c r="X18" s="31"/>
+      <c r="Y18" s="31"/>
+      <c r="Z18" s="30"/>
+      <c r="AA18" s="31"/>
+      <c r="AB18" s="31"/>
+      <c r="AC18" s="31"/>
+      <c r="AD18" s="31"/>
+      <c r="AE18" s="31"/>
+      <c r="AF18" s="31"/>
     </row>
     <row r="19" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21">
+      <c r="A19" s="15">
         <f>A17+1</f>
         <v>13</v>
       </c>
-      <c r="B19" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="39" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="I19" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="J19" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="K19" s="32"/>
-      <c r="L19" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="M19" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="N19" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="O19" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="P19" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q19" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="R19" s="32"/>
-      <c r="S19" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="T19" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="U19" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="V19" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="W19" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="X19" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y19" s="32"/>
-      <c r="Z19" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA19" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="AB19" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="AC19" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="AD19" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE19" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF19" s="32"/>
+      <c r="B19" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="J19" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="K19" s="26"/>
+      <c r="L19" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="M19" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="N19" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="O19" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="P19" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q19" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="R19" s="26"/>
+      <c r="S19" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="T19" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="U19" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="V19" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="W19" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="X19" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y19" s="26"/>
+      <c r="Z19" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA19" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB19" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC19" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD19" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE19" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF19" s="26"/>
     </row>
     <row r="20" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21">
+      <c r="A20" s="15">
         <f>A19+1</f>
         <v>14</v>
       </c>
-      <c r="B20" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="H20" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="I20" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="J20" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="K20" s="32"/>
-      <c r="L20" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="M20" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="N20" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="O20" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="P20" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q20" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="R20" s="32"/>
-      <c r="S20" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="T20" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="U20" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="V20" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="W20" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="X20" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y20" s="32"/>
-      <c r="Z20" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA20" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB20" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC20" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="AD20" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE20" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="AF20" s="32"/>
+      <c r="B20" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="J20" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="K20" s="26"/>
+      <c r="L20" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="M20" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="N20" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="O20" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="P20" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q20" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="R20" s="26"/>
+      <c r="S20" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="T20" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="U20" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="V20" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="W20" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="X20" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y20" s="26"/>
+      <c r="Z20" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA20" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB20" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC20" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD20" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE20" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF20" s="26"/>
     </row>
     <row r="21" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21">
+      <c r="A21" s="15">
         <f>A20+1</f>
         <v>15</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="H21" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="I21" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="J21" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="K21" s="30"/>
-      <c r="L21" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="M21" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="N21" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="O21" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="P21" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q21" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="R21" s="30"/>
-      <c r="S21" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="T21" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="U21" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="V21" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="W21" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="X21" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y21" s="30"/>
-      <c r="Z21" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA21" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="AB21" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="AC21" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD21" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE21" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF21" s="30"/>
+      <c r="F21" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="H21" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" s="24"/>
+      <c r="L21" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="M21" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="N21" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="O21" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="P21" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q21" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="R21" s="24"/>
+      <c r="S21" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="T21" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="U21" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="V21" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="W21" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="X21" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y21" s="24"/>
+      <c r="Z21" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA21" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB21" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC21" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD21" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE21" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF21" s="24"/>
     </row>
     <row r="22" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21">
+      <c r="A22" s="15">
         <f>A21+1</f>
         <v>16</v>
       </c>
-      <c r="B22" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="24" t="s">
+      <c r="B22" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="H22" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F22" s="24" t="s">
+      <c r="I22" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="24" t="s">
+      <c r="J22" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="H22" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="J22" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="K22" s="40"/>
-      <c r="L22" s="24" t="s">
+      <c r="K22" s="34"/>
+      <c r="L22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="M22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="N22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="O22" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="M22" s="24" t="s">
+      <c r="P22" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="N22" s="24" t="s">
+      <c r="Q22" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="O22" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="P22" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q22" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="R22" s="40"/>
-      <c r="S22" s="24" t="s">
+      <c r="R22" s="34"/>
+      <c r="S22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="T22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="U22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="V22" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="T22" s="24" t="s">
+      <c r="W22" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="U22" s="24" t="s">
+      <c r="X22" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="V22" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="W22" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="X22" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="Y22" s="40"/>
-      <c r="Z22" s="24" t="s">
+      <c r="Y22" s="34"/>
+      <c r="Z22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB22" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC22" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="AA22" s="24" t="s">
+      <c r="AD22" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="AB22" s="24" t="s">
+      <c r="AE22" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="AC22" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD22" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE22" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="AF22" s="40"/>
+      <c r="AF22" s="34"/>
     </row>
     <row r="23" spans="1:32" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="41">
+      <c r="A23" s="35">
         <f>A22+1</f>
         <v>17</v>
       </c>
-      <c r="B23" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="D23" s="23" t="s">
+      <c r="B23" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="F23" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="G23" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="H23" s="45"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="46"/>
-      <c r="K23" s="47"/>
-      <c r="L23" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="M23" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="N23" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="O23" s="45"/>
-      <c r="P23" s="46"/>
-      <c r="Q23" s="46"/>
-      <c r="R23" s="47"/>
-      <c r="S23" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="T23" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="U23" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="V23" s="45"/>
-      <c r="W23" s="46"/>
-      <c r="X23" s="46"/>
-      <c r="Y23" s="47"/>
-      <c r="Z23" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA23" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB23" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC23" s="45"/>
-      <c r="AD23" s="46"/>
-      <c r="AE23" s="46"/>
-      <c r="AF23" s="47"/>
+      <c r="C23" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="G23" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="H23" s="38"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="M23" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="N23" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="O23" s="38"/>
+      <c r="P23" s="39"/>
+      <c r="Q23" s="39"/>
+      <c r="R23" s="40"/>
+      <c r="S23" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="T23" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="U23" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="V23" s="38"/>
+      <c r="W23" s="39"/>
+      <c r="X23" s="39"/>
+      <c r="Y23" s="40"/>
+      <c r="Z23" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA23" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB23" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC23" s="38"/>
+      <c r="AD23" s="39"/>
+      <c r="AE23" s="39"/>
+      <c r="AF23" s="40"/>
     </row>
     <row r="24" spans="1:32" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>

<commit_message>
đang code dở thuật toán
</commit_message>
<xml_diff>
--- a/Template/DV3.xlsx
+++ b/Template/DV3.xlsx
@@ -3886,6 +3886,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:AF24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -3894,7 +3897,30 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="6" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="18.75" x14ac:dyDescent="0.3">
@@ -3949,14 +3975,14 @@
       </c>
       <c r="F2" s="5">
         <f>E4</f>
-        <v>43634</v>
+        <v>43633</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>2</v>
       </c>
       <c r="H2" s="5">
         <f>J4</f>
-        <v>43639</v>
+        <v>43638</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -3966,14 +3992,14 @@
       </c>
       <c r="M2" s="5">
         <f>L4</f>
-        <v>43641</v>
+        <v>43640</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>2</v>
       </c>
       <c r="O2" s="5">
         <f>Q4</f>
-        <v>43646</v>
+        <v>43645</v>
       </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
@@ -3983,14 +4009,14 @@
       </c>
       <c r="T2" s="5">
         <f>S4</f>
-        <v>43648</v>
+        <v>43647</v>
       </c>
       <c r="U2" s="6" t="s">
         <v>2</v>
       </c>
       <c r="V2" s="5">
         <f>X4</f>
-        <v>43653</v>
+        <v>43652</v>
       </c>
       <c r="W2" s="5"/>
       <c r="X2" s="5"/>
@@ -4000,14 +4026,14 @@
       </c>
       <c r="AA2" s="5">
         <f>Z4</f>
-        <v>43655</v>
+        <v>43654</v>
       </c>
       <c r="AB2" s="6" t="s">
         <v>2</v>
       </c>
       <c r="AC2" s="5">
         <f>AE4</f>
-        <v>43660</v>
+        <v>43659</v>
       </c>
       <c r="AD2" s="5"/>
       <c r="AE2" s="5"/>
@@ -4061,115 +4087,115 @@
         <v>6</v>
       </c>
       <c r="E4" s="9">
-        <v>43634</v>
+        <v>43633</v>
       </c>
       <c r="F4" s="9">
         <f t="shared" ref="F4:AF4" si="0">E4+1</f>
-        <v>43635</v>
+        <v>43634</v>
       </c>
       <c r="G4" s="9">
         <f t="shared" si="0"/>
-        <v>43636</v>
+        <v>43635</v>
       </c>
       <c r="H4" s="9">
         <f t="shared" si="0"/>
-        <v>43637</v>
+        <v>43636</v>
       </c>
       <c r="I4" s="9">
         <f t="shared" si="0"/>
-        <v>43638</v>
+        <v>43637</v>
       </c>
       <c r="J4" s="9">
         <f t="shared" si="0"/>
-        <v>43639</v>
+        <v>43638</v>
       </c>
       <c r="K4" s="9">
         <f t="shared" si="0"/>
-        <v>43640</v>
+        <v>43639</v>
       </c>
       <c r="L4" s="9">
         <f t="shared" si="0"/>
-        <v>43641</v>
+        <v>43640</v>
       </c>
       <c r="M4" s="9">
         <f t="shared" si="0"/>
-        <v>43642</v>
+        <v>43641</v>
       </c>
       <c r="N4" s="9">
         <f t="shared" si="0"/>
-        <v>43643</v>
+        <v>43642</v>
       </c>
       <c r="O4" s="9">
         <f t="shared" si="0"/>
-        <v>43644</v>
+        <v>43643</v>
       </c>
       <c r="P4" s="9">
         <f t="shared" si="0"/>
-        <v>43645</v>
+        <v>43644</v>
       </c>
       <c r="Q4" s="9">
         <f t="shared" si="0"/>
-        <v>43646</v>
+        <v>43645</v>
       </c>
       <c r="R4" s="9">
         <f t="shared" si="0"/>
-        <v>43647</v>
+        <v>43646</v>
       </c>
       <c r="S4" s="9">
         <f t="shared" si="0"/>
-        <v>43648</v>
+        <v>43647</v>
       </c>
       <c r="T4" s="9">
         <f t="shared" si="0"/>
-        <v>43649</v>
+        <v>43648</v>
       </c>
       <c r="U4" s="9">
         <f t="shared" si="0"/>
-        <v>43650</v>
+        <v>43649</v>
       </c>
       <c r="V4" s="9">
         <f t="shared" si="0"/>
-        <v>43651</v>
+        <v>43650</v>
       </c>
       <c r="W4" s="9">
         <f t="shared" si="0"/>
-        <v>43652</v>
+        <v>43651</v>
       </c>
       <c r="X4" s="9">
         <f t="shared" si="0"/>
-        <v>43653</v>
+        <v>43652</v>
       </c>
       <c r="Y4" s="9">
         <f t="shared" si="0"/>
-        <v>43654</v>
+        <v>43653</v>
       </c>
       <c r="Z4" s="9">
         <f t="shared" si="0"/>
-        <v>43655</v>
+        <v>43654</v>
       </c>
       <c r="AA4" s="9">
         <f t="shared" si="0"/>
-        <v>43656</v>
+        <v>43655</v>
       </c>
       <c r="AB4" s="9">
         <f t="shared" si="0"/>
-        <v>43657</v>
+        <v>43656</v>
       </c>
       <c r="AC4" s="9">
         <f t="shared" si="0"/>
-        <v>43658</v>
+        <v>43657</v>
       </c>
       <c r="AD4" s="9">
         <f t="shared" si="0"/>
-        <v>43659</v>
+        <v>43658</v>
       </c>
       <c r="AE4" s="9">
         <f t="shared" si="0"/>
-        <v>43660</v>
+        <v>43659</v>
       </c>
       <c r="AF4" s="9">
         <f t="shared" si="0"/>
-        <v>43661</v>
+        <v>43660</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
@@ -5692,6 +5718,6 @@
     <mergeCell ref="D4:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="55" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>